<commit_message>
convert VSI to vector of 6 length
</commit_message>
<xml_diff>
--- a/ComponentParameterGrid.xlsx
+++ b/ComponentParameterGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\GenUnit2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB2863D-7AC3-4468-A395-BBCF074F5376}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B8681F-AE3E-4D45-A4B8-6DF9DE2A4D3C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7920" xr2:uid="{1CF92AFD-01AD-497D-A694-A6978AB197A2}"/>
   </bookViews>
@@ -271,9 +271,6 @@
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -284,9 +281,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -310,6 +304,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -627,7 +627,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,429 +636,429 @@
     <col min="4" max="4" width="1.28515625" customWidth="1"/>
     <col min="5" max="5" width="6.5703125" customWidth="1"/>
     <col min="8" max="8" width="1.140625" customWidth="1"/>
-    <col min="9" max="9" width="7.7109375" style="13" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" style="11" customWidth="1"/>
     <col min="12" max="12" width="1.28515625" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" style="13"/>
+    <col min="13" max="13" width="13.85546875" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="1" t="s">
+      <c r="C1" s="20"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="1" t="s">
+      <c r="G1" s="20"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="1" t="s">
+      <c r="K1" s="20"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="O1" s="1"/>
+      <c r="O1" s="20"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="7" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="11" t="s">
+      <c r="H2" s="3"/>
+      <c r="I2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L2" s="9"/>
-      <c r="M2" s="11" t="s">
+      <c r="L2" s="7"/>
+      <c r="M2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="N2" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="O2" s="8" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="8" t="s">
+      <c r="D3" s="3"/>
+      <c r="E3" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="8" t="s">
+      <c r="H3" s="3"/>
+      <c r="I3" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="J3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="K3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="4"/>
-      <c r="M3" s="8" t="s">
+      <c r="L3" s="3"/>
+      <c r="M3" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="N3" s="20" t="s">
+      <c r="N3" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="2"/>
+      <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="14" t="s">
+      <c r="A4" s="21"/>
+      <c r="B4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="15" t="s">
+      <c r="D4" s="3"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="14" t="s">
+      <c r="H4" s="3"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="K4" s="14" t="s">
+      <c r="K4" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="L4" s="4"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="15" t="s">
+      <c r="L4" s="3"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="O4" s="15" t="s">
+      <c r="O4" s="13" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="14" t="s">
+      <c r="A5" s="21"/>
+      <c r="B5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="15" t="s">
+      <c r="D5" s="3"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="14" t="s">
+      <c r="G5" s="1"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="K5" s="14" t="s">
+      <c r="K5" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="L5" s="4"/>
-      <c r="M5" s="7" t="s">
+      <c r="L5" s="3"/>
+      <c r="M5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="N5" s="14" t="s">
+      <c r="N5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="O5" s="14" t="s">
+      <c r="O5" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="20" t="s">
+      <c r="D6" s="3"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="8" t="s">
+      <c r="G6" s="1"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="K6" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="L6" s="4"/>
-      <c r="M6" s="12"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="10"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="15" t="s">
+      <c r="A7" s="21"/>
+      <c r="B7" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="14" t="s">
+      <c r="D7" s="3"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="14" t="s">
+      <c r="H7" s="3"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="K7" s="14" t="s">
+      <c r="K7" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="L7" s="4"/>
-      <c r="M7" s="12"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="10"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="18" t="s">
+      <c r="A8" s="21"/>
+      <c r="B8" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="18" t="s">
+      <c r="D8" s="3"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="12"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="15" t="s">
+      <c r="A9" s="21"/>
+      <c r="B9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="18" t="s">
+      <c r="D9" s="3"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="G9" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="4"/>
-      <c r="I9" s="12"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="20" t="s">
+      <c r="A10" s="21"/>
+      <c r="B10" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="14" t="s">
+      <c r="D10" s="3"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="12"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="18" t="s">
+      <c r="A11" s="21"/>
+      <c r="B11" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="20" t="s">
+      <c r="D11" s="3"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="20" t="s">
+      <c r="G11" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="12"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="15" t="s">
+      <c r="A12" s="21"/>
+      <c r="B12" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="8" t="s">
+      <c r="D12" s="3"/>
+      <c r="E12" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="12"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="15" t="s">
+      <c r="A13" s="21"/>
+      <c r="B13" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="14" t="s">
+      <c r="D13" s="3"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="H13" s="4"/>
-      <c r="I13" s="12"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="20" t="s">
+      <c r="A14" s="21"/>
+      <c r="B14" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="18" t="s">
+      <c r="D14" s="3"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="12"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="20" t="s">
+      <c r="A15" s="21"/>
+      <c r="B15" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="18" t="s">
+      <c r="A16" s="21"/>
+      <c r="B16" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
+      <c r="A18" s="14"/>
       <c r="B18" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
+      <c r="A19" s="15"/>
       <c r="B19" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
+      <c r="A20" s="17"/>
       <c r="B20" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
+      <c r="A21" s="19"/>
       <c r="B21" t="s">
         <v>47</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A16"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="J1:K1"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="E3:E11"/>
     <mergeCell ref="E12:E14"/>
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="I3:I5"/>
     <mergeCell ref="M3:M4"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A16"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add GENSAL and update its signal names to match templates
</commit_message>
<xml_diff>
--- a/ComponentParameterGrid.xlsx
+++ b/ComponentParameterGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\GenUnit2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B8681F-AE3E-4D45-A4B8-6DF9DE2A4D3C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021288C0-A22F-4EC6-ABA7-1AE11741DDA3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7920" xr2:uid="{1CF92AFD-01AD-497D-A694-A6978AB197A2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="50">
   <si>
     <t>PMECH</t>
   </si>
@@ -175,6 +175,12 @@
   </si>
   <si>
     <t>Does not exist in template, however it is needed by other blocks</t>
+  </si>
+  <si>
+    <t>converted from RealOutput to Real</t>
+  </si>
+  <si>
+    <t>removed or commented out</t>
   </si>
 </sst>
 </file>
@@ -190,7 +196,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,6 +224,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -269,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -310,6 +328,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05F88B56-328B-4552-8712-5B07DA59822A}">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,7 +837,7 @@
       <c r="A6" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="13" t="s">
@@ -842,7 +864,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="21"/>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="13" t="s">
@@ -869,7 +891,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="21"/>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="23" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="16" t="s">
@@ -888,7 +910,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="21"/>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="12" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="13" t="s">
@@ -907,7 +929,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="12" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="13" t="s">
@@ -926,7 +948,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="21"/>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="23" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="16" t="s">
@@ -945,10 +967,10 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="21"/>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="12" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="3"/>
@@ -966,7 +988,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="21"/>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="13" t="s">
@@ -985,7 +1007,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="13" t="s">
@@ -1002,7 +1024,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="21"/>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="24" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="16" t="s">
@@ -1013,7 +1035,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="21"/>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="23" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="16" t="s">
@@ -1044,6 +1066,18 @@
       <c r="A21" s="19"/>
       <c r="B21" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="22"/>
+      <c r="B22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="25"/>
+      <c r="B23" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add GENROU, matches template
</commit_message>
<xml_diff>
--- a/ComponentParameterGrid.xlsx
+++ b/ComponentParameterGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\GenUnit2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021288C0-A22F-4EC6-ABA7-1AE11741DDA3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A44E278A-EC0E-4F5B-9276-CCD466B363A2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7920" xr2:uid="{1CF92AFD-01AD-497D-A694-A6978AB197A2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="50">
   <si>
     <t>PMECH</t>
   </si>
@@ -649,7 +649,7 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,7 +840,7 @@
       <c r="B6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="3"/>
@@ -867,7 +867,7 @@
       <c r="B7" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="3"/>
@@ -894,7 +894,7 @@
       <c r="B8" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="23" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="3"/>
@@ -913,7 +913,7 @@
       <c r="B9" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="3"/>
@@ -932,7 +932,7 @@
       <c r="B10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="12" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="3"/>
@@ -951,7 +951,7 @@
       <c r="B11" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="23" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="3"/>
@@ -991,7 +991,7 @@
       <c r="B13" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="12" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="3"/>
@@ -1010,7 +1010,7 @@
       <c r="B14" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="3"/>
@@ -1038,7 +1038,7 @@
       <c r="B16" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="23" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="3"/>

</xml_diff>